<commit_message>
Fechas de pago y numero de contrato
</commit_message>
<xml_diff>
--- a/static/documentos/reporte_0.xlsx
+++ b/static/documentos/reporte_0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador.SERVIDOR-HP.002\Desktop\Nueva carpeta (2)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador.SERVIDOR-HP.002\Desktop\Nueva carpeta\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -114,15 +114,6 @@
     <t>Soporte que respalda:</t>
   </si>
   <si>
-    <t>Fin:</t>
-  </si>
-  <si>
-    <t>Inicio:</t>
-  </si>
-  <si>
-    <t>Periodo de adquisición de bien o servicio</t>
-  </si>
-  <si>
     <t>Numero de pagos a efectuar en el presente reporte:</t>
   </si>
   <si>
@@ -774,6 +765,15 @@
   </si>
   <si>
     <t>Coordinador administrativo</t>
+  </si>
+  <si>
+    <t>Fechas del reporte</t>
+  </si>
+  <si>
+    <t>Pago:</t>
+  </si>
+  <si>
+    <t>Cargue:</t>
   </si>
 </sst>
 </file>
@@ -2418,7 +2418,7 @@
       <c r="H6" s="86"/>
       <c r="I6" s="87"/>
       <c r="J6" s="122" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="K6" s="123"/>
       <c r="L6" s="123"/>
@@ -2432,14 +2432,14 @@
       <c r="C7" s="96"/>
       <c r="D7" s="96"/>
       <c r="E7" s="31" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F7" s="85"/>
       <c r="G7" s="86"/>
       <c r="H7" s="86"/>
       <c r="I7" s="87"/>
       <c r="J7" s="119" t="s">
-        <v>29</v>
+        <v>238</v>
       </c>
       <c r="K7" s="120"/>
       <c r="L7" s="120"/>
@@ -2453,21 +2453,21 @@
       <c r="C8" s="99"/>
       <c r="D8" s="99"/>
       <c r="E8" s="74" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F8" s="75"/>
       <c r="G8" s="34"/>
       <c r="H8" s="76" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I8" s="77"/>
       <c r="J8" s="25" t="s">
-        <v>28</v>
+        <v>239</v>
       </c>
       <c r="K8" s="60"/>
       <c r="L8" s="78"/>
       <c r="M8" s="81" t="s">
-        <v>27</v>
+        <v>240</v>
       </c>
       <c r="N8" s="82"/>
       <c r="O8" s="60"/>
@@ -2502,7 +2502,7 @@
       </c>
       <c r="K10" s="70"/>
       <c r="L10" s="72" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="M10" s="68" t="s">
         <v>10</v>
@@ -2569,29 +2569,29 @@
     </row>
     <row r="15" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="35" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C15" s="36"/>
       <c r="D15" s="36"/>
       <c r="E15" s="36"/>
       <c r="F15" s="37" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G15" s="38"/>
       <c r="H15" s="39"/>
       <c r="I15" s="37" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="J15" s="40"/>
       <c r="K15" s="40"/>
       <c r="L15" s="41"/>
       <c r="M15" s="103" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="N15" s="104"/>
       <c r="O15" s="104"/>
       <c r="P15" s="62" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="21" x14ac:dyDescent="0.35">
@@ -2641,7 +2641,7 @@
       <c r="K18" s="47"/>
       <c r="L18" s="48"/>
       <c r="M18" s="105" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="N18" s="106"/>
       <c r="O18" s="106"/>
@@ -2651,18 +2651,18 @@
     </row>
     <row r="19" spans="2:16" ht="21" x14ac:dyDescent="0.35">
       <c r="B19" s="57" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C19" s="58"/>
       <c r="D19" s="58"/>
       <c r="E19" s="59"/>
       <c r="F19" s="57" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G19" s="58"/>
       <c r="H19" s="58"/>
       <c r="I19" s="57" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="J19" s="58"/>
       <c r="K19" s="58"/>
@@ -2766,10 +2766,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C1" t="b">
         <f t="shared" ref="C1:C43" si="0">EXACT(A1,B1)</f>
@@ -2781,10 +2781,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C2" t="b">
         <f t="shared" si="0"/>
@@ -2796,10 +2796,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C3" t="b">
         <f t="shared" si="0"/>
@@ -2811,10 +2811,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C4" t="b">
         <f t="shared" si="0"/>
@@ -2826,10 +2826,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C5" t="b">
         <f t="shared" si="0"/>
@@ -2841,10 +2841,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C6" t="b">
         <f t="shared" si="0"/>
@@ -2856,10 +2856,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C7" t="b">
         <f t="shared" si="0"/>
@@ -2871,10 +2871,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C8" t="b">
         <f t="shared" si="0"/>
@@ -2886,10 +2886,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C9" t="b">
         <f t="shared" si="0"/>
@@ -2901,10 +2901,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C10" t="b">
         <f t="shared" si="0"/>
@@ -2916,10 +2916,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C11" t="b">
         <f t="shared" si="0"/>
@@ -2931,10 +2931,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C12" t="b">
         <f t="shared" si="0"/>
@@ -2946,10 +2946,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C13" t="b">
         <f t="shared" si="0"/>
@@ -2961,10 +2961,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C14" t="b">
         <f t="shared" si="0"/>
@@ -2976,10 +2976,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C15" t="b">
         <f t="shared" si="0"/>
@@ -2991,10 +2991,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C16" t="b">
         <f t="shared" si="0"/>
@@ -3006,10 +3006,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C17" t="b">
         <f t="shared" si="0"/>
@@ -3021,10 +3021,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C18" t="b">
         <f t="shared" si="0"/>
@@ -3036,10 +3036,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C19" t="b">
         <f t="shared" si="0"/>
@@ -3051,10 +3051,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C20" t="b">
         <f t="shared" si="0"/>
@@ -3066,10 +3066,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C21" t="b">
         <f t="shared" si="0"/>
@@ -3081,10 +3081,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C22" t="b">
         <f t="shared" si="0"/>
@@ -3111,10 +3111,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C24" t="b">
         <f t="shared" si="0"/>
@@ -3126,10 +3126,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C25" t="b">
         <f t="shared" si="0"/>
@@ -3141,10 +3141,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C26" t="b">
         <f t="shared" si="0"/>
@@ -3156,10 +3156,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C27" t="b">
         <f t="shared" si="0"/>
@@ -3186,10 +3186,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C29" t="b">
         <f t="shared" si="0"/>
@@ -3201,10 +3201,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C30" t="b">
         <f t="shared" si="0"/>
@@ -3216,10 +3216,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C31" t="b">
         <f t="shared" si="0"/>
@@ -3231,10 +3231,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C32" t="b">
         <f t="shared" si="0"/>
@@ -3246,10 +3246,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C33" t="b">
         <f t="shared" si="0"/>
@@ -3261,10 +3261,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C34" t="b">
         <f t="shared" si="0"/>
@@ -3276,10 +3276,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C35" t="b">
         <f t="shared" si="0"/>
@@ -3291,10 +3291,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C36" t="b">
         <f t="shared" si="0"/>
@@ -3306,10 +3306,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C37" t="b">
         <f t="shared" si="0"/>
@@ -3321,10 +3321,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C38" t="b">
         <f t="shared" si="0"/>
@@ -3336,10 +3336,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C39" t="b">
         <f t="shared" si="0"/>
@@ -3351,10 +3351,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C40" t="b">
         <f t="shared" si="0"/>
@@ -3366,10 +3366,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C41" t="b">
         <f t="shared" si="0"/>
@@ -3381,10 +3381,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C42" t="b">
         <f t="shared" si="0"/>
@@ -3396,10 +3396,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C43" t="b">
         <f t="shared" si="0"/>
@@ -3438,28 +3438,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="E1" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="G1" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="H1" s="22" t="s">
         <v>188</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3765,13 +3765,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3779,7 +3779,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3790,7 +3790,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3801,7 +3801,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C4">
         <v>6</v>
@@ -3812,7 +3812,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C5">
         <v>7</v>
@@ -3823,7 +3823,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -3834,7 +3834,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -3845,7 +3845,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -3856,7 +3856,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C9">
         <v>12</v>
@@ -3867,7 +3867,7 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C10">
         <v>13</v>
@@ -3878,7 +3878,7 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C11">
         <v>14</v>
@@ -3889,7 +3889,7 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C12">
         <v>19</v>
@@ -3900,7 +3900,7 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C13">
         <v>23</v>
@@ -3911,7 +3911,7 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C14">
         <v>32</v>
@@ -3922,7 +3922,7 @@
         <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C15">
         <v>40</v>
@@ -3933,7 +3933,7 @@
         <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C16">
         <v>41</v>
@@ -3944,7 +3944,7 @@
         <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C17">
         <v>51</v>
@@ -3955,7 +3955,7 @@
         <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C18">
         <v>52</v>
@@ -3966,7 +3966,7 @@
         <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C19">
         <v>58</v>
@@ -3977,7 +3977,7 @@
         <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C20">
         <v>60</v>
@@ -3988,7 +3988,7 @@
         <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C21">
         <v>61</v>
@@ -3999,7 +3999,7 @@
         <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C22">
         <v>62</v>
@@ -4010,7 +4010,7 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C23">
         <v>63</v>
@@ -4021,7 +4021,7 @@
         <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C24">
         <v>65</v>
@@ -4032,7 +4032,7 @@
         <v>76</v>
       </c>
       <c r="B25" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C25">
         <v>76</v>
@@ -4043,7 +4043,7 @@
         <v>90</v>
       </c>
       <c r="B26" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C26">
         <v>90</v>
@@ -4054,7 +4054,7 @@
         <v>283</v>
       </c>
       <c r="B27" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C27">
         <v>283</v>
@@ -4065,7 +4065,7 @@
         <v>289</v>
       </c>
       <c r="B28" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C28">
         <v>289</v>
@@ -4076,7 +4076,7 @@
         <v>292</v>
       </c>
       <c r="B29" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C29">
         <v>292</v>
@@ -4087,7 +4087,7 @@
         <v>296</v>
       </c>
       <c r="B30" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C30">
         <v>296</v>
@@ -4125,25 +4125,25 @@
         <v>4</v>
       </c>
       <c r="C1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>35</v>
       </c>
       <c r="J1" s="16" t="s">
         <v>1</v>
@@ -4152,10 +4152,10 @@
         <v>5</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
@@ -4163,37 +4163,37 @@
         <v>1098630887</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D2" s="19">
         <v>3132608629</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G2" s="20" t="s">
         <v>24</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J2" s="19" t="s">
         <v>9</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="M2" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
@@ -4201,37 +4201,37 @@
         <v>1099548034</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D3" s="6">
         <v>3162707702</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L3" s="10">
         <v>81489704072</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
@@ -4239,37 +4239,37 @@
         <v>1057587077</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D4" s="6">
         <v>3134165999</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L4" s="11">
         <v>596382614</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
@@ -4277,37 +4277,37 @@
         <v>1098639059</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D5" s="6">
         <v>3506814958</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
@@ -4315,37 +4315,37 @@
         <v>1098703596</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D6" s="6">
         <v>3209409025</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
@@ -4353,37 +4353,37 @@
         <v>91492568</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D7" s="6">
         <v>3144254673</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L7" s="9">
         <v>29768335611</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
@@ -4391,37 +4391,37 @@
         <v>23498533</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D8" s="6">
         <v>3165554894</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
@@ -4429,37 +4429,37 @@
         <v>1095794422</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D9" s="6">
         <v>3168746386</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
@@ -4467,37 +4467,37 @@
         <v>74189878</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D10" s="6">
         <v>3125411780</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L10" s="12">
         <v>36363295317</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
@@ -4505,37 +4505,37 @@
         <v>28161949</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D11" s="6">
         <v>3112762013</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
@@ -4543,37 +4543,37 @@
         <v>63535545</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D12" s="6">
         <v>3173650121</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L12" s="9">
         <v>46170368321</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
@@ -4581,37 +4581,37 @@
         <v>37752780</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D13" s="6">
         <v>3182617356</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
@@ -4619,37 +4619,37 @@
         <v>63506284</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D14" s="6">
         <v>3156298493</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L14" s="9">
         <v>29148916584</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
@@ -4663,31 +4663,31 @@
         <v>3123556832</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L15" s="14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
@@ -4695,37 +4695,37 @@
         <v>1095812851</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D16" s="6">
         <v>3106692290</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
@@ -4733,37 +4733,37 @@
         <v>1095821501</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D17" s="6">
         <v>3154668200</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
@@ -4771,37 +4771,37 @@
         <v>74130395</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D18" s="6">
         <v>3124580548</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
@@ -4809,37 +4809,37 @@
         <v>13541294</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D19" s="6">
         <v>3175709009</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
@@ -4847,37 +4847,37 @@
         <v>74381668</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D20" s="6">
         <v>3112841130</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
@@ -4885,37 +4885,37 @@
         <v>1099549339</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D21" s="6">
         <v>3184249504</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="I21" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
@@ -4923,37 +4923,37 @@
         <v>1101686236</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D22" s="6">
         <v>3102876566</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="I22" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
@@ -4961,37 +4961,37 @@
         <v>63557785</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D23" s="6">
         <v>3185645912</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J23" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L23" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
@@ -4999,37 +4999,37 @@
         <v>1100894181</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D24" s="6">
         <v>3005765923</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J24" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L24" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
@@ -5037,37 +5037,37 @@
         <v>46457774</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D25" s="6">
         <v>3202332188</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="L25" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
@@ -5075,37 +5075,37 @@
         <v>1065644811</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D26" s="6">
         <v>3004660558</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L26" s="9">
         <v>52357836590</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
@@ -5113,37 +5113,37 @@
         <v>37750502</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D27" s="6">
         <v>3003632198</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L27" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
@@ -5151,37 +5151,37 @@
         <v>1098639462</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D28" s="6">
         <v>3209044509</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J28" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="M28" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
@@ -5189,37 +5189,37 @@
         <v>91493407</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D29" s="6">
         <v>3162253773</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J29" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L29" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
@@ -5227,37 +5227,37 @@
         <v>74081102</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D30" s="6">
         <v>3114630069</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J30" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="M30" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
@@ -5265,37 +5265,37 @@
         <v>63512053</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D31" s="6">
         <v>3158707945</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J31" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="L31" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="M31" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
@@ -5303,37 +5303,37 @@
         <v>1098639373</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D32" s="6">
         <v>3004144721</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L32" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="M32" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
@@ -5341,37 +5341,37 @@
         <v>1099552826</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D33" s="6">
         <v>3219922005</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F33" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="I33" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J33" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L33" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="M33" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
@@ -5379,37 +5379,37 @@
         <v>13872207</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D34" s="6">
         <v>3165763599</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J34" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="M34" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
@@ -5417,37 +5417,37 @@
         <v>63348229</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D35" s="6">
         <v>3102262348</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J35" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L35" s="9">
         <v>68000028081</v>
       </c>
       <c r="M35" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
@@ -5455,37 +5455,37 @@
         <v>1125228826</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D36" s="6">
         <v>3164169493</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F36" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="I36" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J36" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K36" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L36" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="M36" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
@@ -5493,37 +5493,37 @@
         <v>1005148938</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D37" s="6">
         <v>3166088078</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F37" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I37" s="6" t="s">
         <v>132</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>135</v>
       </c>
       <c r="J37" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L37" s="12" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="M37" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
@@ -5531,37 +5531,37 @@
         <v>63542893</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D38" s="6">
         <v>3138105797</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J38" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L38" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="M38" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
@@ -5569,37 +5569,37 @@
         <v>63510325</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D39" s="6">
         <v>3154269363</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J39" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K39" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L39" s="12" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="M39" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
@@ -5607,37 +5607,37 @@
         <v>63542491</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D40" s="6">
         <v>3202152771</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J40" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K40" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L40" s="11">
         <v>392010843</v>
       </c>
       <c r="M40" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
@@ -5645,37 +5645,37 @@
         <v>1140874058</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D41" s="6">
         <v>3006602943</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F41" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="I41" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J41" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L41" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M41" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
@@ -5683,37 +5683,37 @@
         <v>1057305014</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D42" s="6">
         <v>3137816328</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L42" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="M42" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>